<commit_message>
new feature files for update and invalid tests added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/userData.xlsx
+++ b/src/test/resources/testData/userData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1cd4c7df07e554a1/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{6B46D770-18E6-4EBA-BA9D-28893922483D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E70B718-23B0-4362-AE91-1183EF1E89EB}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{4CBE65F6-6E86-41E8-A21B-3A7F35A59C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E90032C-46F2-4F94-9D64-DF70BBF30407}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{EBE3E444-D642-44F6-9A91-CEF4C2359EC4}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{EBE3E444-D642-44F6-9A91-CEF4C2359EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="userData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>plotNumber</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>invalidUserEmail</t>
+  </si>
+  <si>
+    <t>updateUser</t>
   </si>
 </sst>
 </file>
@@ -961,7 +964,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,61 +1053,16 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>9265</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3">
-        <v>2222222223</v>
-      </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
       <c r="B4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>9265</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4">
-        <v>2222222223</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>